<commit_message>
adding mr_wilson attempting to fix Mr_Stone
</commit_message>
<xml_diff>
--- a/36_Mr_Stone/Mr_Stone_Data.xlsx
+++ b/36_Mr_Stone/Mr_Stone_Data.xlsx
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:D58"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -593,7 +593,7 @@
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" thickBot="1">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45.75" thickBot="1">
+    <row r="2" spans="1:4" ht="30.75" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -649,7 +649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45.75" thickBot="1">
+    <row r="5" spans="1:4" ht="30.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -938,7 +938,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="4">
-        <v>7.3</v>
+        <v>7.23</v>
       </c>
       <c r="C29" s="4">
         <v>7.45</v>
@@ -952,7 +952,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="4">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C30" s="4">
         <v>37</v>

</xml_diff>

<commit_message>
Making Changes to Lab 36
</commit_message>
<xml_diff>
--- a/36_Mr_Stone/Mr_Stone_Data.xlsx
+++ b/36_Mr_Stone/Mr_Stone_Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="50">
   <si>
     <t>Variable</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Now</t>
+  </si>
+  <si>
+    <t>Didn't try to mess around with IV ion concentrations and delivery options. We'll leave that up to the students.</t>
   </si>
 </sst>
 </file>
@@ -191,12 +194,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -263,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -286,6 +295,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -796,7 +809,7 @@
         <v>26</v>
       </c>
       <c r="B17" s="4">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C17" s="4">
         <v>37</v>
@@ -810,7 +823,7 @@
         <v>27</v>
       </c>
       <c r="B18" s="4">
-        <v>7.3</v>
+        <v>7.23</v>
       </c>
       <c r="C18" s="4">
         <v>7.45</v>
@@ -824,7 +837,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="4">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C19" s="4">
         <v>35</v>
@@ -838,7 +851,7 @@
         <v>31</v>
       </c>
       <c r="B20" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C20" s="4">
         <v>26</v>
@@ -895,7 +908,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C25" s="4">
         <v>26</v>
@@ -909,7 +922,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C26" s="4">
         <v>11</v>
@@ -1167,9 +1180,7 @@
       <c r="B48" s="4">
         <v>146</v>
       </c>
-      <c r="C48" s="4">
-        <v>157</v>
-      </c>
+      <c r="C48" s="4"/>
       <c r="D48" s="5" t="s">
         <v>15</v>
       </c>
@@ -1181,9 +1192,7 @@
       <c r="B49" s="4">
         <v>4.5</v>
       </c>
-      <c r="C49" s="4">
-        <v>3.9</v>
-      </c>
+      <c r="C49" s="4"/>
       <c r="D49" s="5" t="s">
         <v>15</v>
       </c>
@@ -1195,9 +1204,7 @@
       <c r="B50" s="4">
         <v>122</v>
       </c>
-      <c r="C50" s="4">
-        <v>104</v>
-      </c>
+      <c r="C50" s="4"/>
       <c r="D50" s="5" t="s">
         <v>15</v>
       </c>
@@ -1209,9 +1216,7 @@
       <c r="B51" s="4">
         <v>21</v>
       </c>
-      <c r="C51" s="4">
-        <v>20</v>
-      </c>
+      <c r="C51" s="4"/>
       <c r="D51" s="5" t="s">
         <v>19</v>
       </c>
@@ -1223,9 +1228,7 @@
       <c r="B52" s="4">
         <v>7.3</v>
       </c>
-      <c r="C52" s="4">
-        <v>6.2</v>
-      </c>
+      <c r="C52" s="4"/>
       <c r="D52" s="5" t="s">
         <v>21</v>
       </c>
@@ -1237,9 +1240,7 @@
       <c r="B53" s="4">
         <v>305</v>
       </c>
-      <c r="C53" s="4">
-        <v>322</v>
-      </c>
+      <c r="C53" s="4"/>
       <c r="D53" s="5" t="s">
         <v>23</v>
       </c>
@@ -1251,9 +1252,7 @@
       <c r="B54" s="4">
         <v>45</v>
       </c>
-      <c r="C54" s="4">
-        <v>41</v>
-      </c>
+      <c r="C54" s="4"/>
       <c r="D54" s="5" t="s">
         <v>25</v>
       </c>
@@ -1265,9 +1264,7 @@
       <c r="B55" s="4">
         <v>36</v>
       </c>
-      <c r="C55" s="4">
-        <v>45</v>
-      </c>
+      <c r="C55" s="4"/>
       <c r="D55" s="5" t="s">
         <v>7</v>
       </c>
@@ -1279,9 +1276,7 @@
       <c r="B56" s="4">
         <v>7.3</v>
       </c>
-      <c r="C56" s="4">
-        <v>7.51</v>
-      </c>
+      <c r="C56" s="4"/>
       <c r="D56" s="5" t="s">
         <v>28</v>
       </c>
@@ -1293,9 +1288,7 @@
       <c r="B57" s="4">
         <v>51</v>
       </c>
-      <c r="C57" s="4">
-        <v>31</v>
-      </c>
+      <c r="C57" s="4"/>
       <c r="D57" s="5" t="s">
         <v>30</v>
       </c>
@@ -1307,16 +1300,25 @@
       <c r="B58" s="4">
         <v>18</v>
       </c>
-      <c r="C58" s="4">
-        <v>40</v>
-      </c>
+      <c r="C58" s="4"/>
       <c r="D58" s="5" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="60" spans="1:4" ht="165">
+      <c r="A60" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="9"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>